<commit_message>
added scripts for numerical experiements
</commit_message>
<xml_diff>
--- a/square_results.xlsx
+++ b/square_results.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="36360" windowHeight="21140" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27000" windowHeight="17540" tabRatio="688" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="square top left extend" sheetId="1" r:id="rId1"/>
     <sheet name="square top left shrink" sheetId="2" r:id="rId2"/>
     <sheet name="square top left small shrink" sheetId="3" r:id="rId3"/>
     <sheet name="L center extend" sheetId="4" r:id="rId4"/>
+    <sheet name="L center shrink" sheetId="5" r:id="rId5"/>
+    <sheet name="annulus corner squish" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="9">
   <si>
     <t>Weierstrass</t>
   </si>
@@ -104,8 +106,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -123,17 +127,19 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1595,6 +1601,2152 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="-2145385880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="l"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10997521685254"/>
+          <c:y val="0.424942430545238"/>
+          <c:w val="0.137307052464167"/>
+          <c:h val="0.142096085277076"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Deviation from Target g</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.051696310664716"/>
+          <c:y val="0.162898936170213"/>
+          <c:w val="0.911267605633803"/>
+          <c:h val="0.75531914893617"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Reverse Polar</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.025</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$E$3:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.138</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.12751</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.11033</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10804</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.10806</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.10821</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Weierstrass</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.025</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$D$3:$D$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.17194</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.07849</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.029308</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.011734</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0060245</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.016382</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Cauchy Green</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.025</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.2982</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2838</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2518</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2368</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2296</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.2262</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2127037768"/>
+        <c:axId val="-2129400824"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2127037768"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Edge</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Length</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.444705588789802"/>
+              <c:y val="0.168882978723404"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2129400824"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2129400824"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Root Mean Squared Deviation </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.74397518492008E-5"/>
+              <c:y val="0.333124582944081"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2127037768"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="l"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.159531502423263"/>
+          <c:y val="0.707999132523689"/>
+          <c:w val="0.179009355958938"/>
+          <c:h val="0.127645635926865"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Error</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> in Euler-Langrange Equation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.051696310664716"/>
+          <c:y val="0.162898936170213"/>
+          <c:w val="0.911267605633803"/>
+          <c:h val="0.75531914893617"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Reverse Polar</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.025</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$H$3:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.04158</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.022643</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0065925</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.001857</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00052412</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00013833</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Weierstrass</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.025</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$G$3:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.055331</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.013615</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0032334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00091378</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00023754</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00025474</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Cauchy Green</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.025</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$I$3:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.13574</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.037339</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0093859</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0023573</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00059104</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.000148</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2146977816"/>
+        <c:axId val="-2146715976"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2146977816"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Edge</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Length</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.444705588789802"/>
+              <c:y val="0.168882978723404"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2146715976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2146715976"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Root Mean Squaredd Error </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.74397518492008E-5"/>
+              <c:y val="0.333124582944081"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2146977816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="l"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.175104022191401"/>
+          <c:y val="0.65715167489657"/>
+          <c:w val="0.153684870095122"/>
+          <c:h val="0.127645635926865"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Elastic Energy</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.051696310664716"/>
+          <c:y val="0.162898936170213"/>
+          <c:w val="0.855505468879587"/>
+          <c:h val="0.75531914893617"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Reverse Polar</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.025</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$H$3:$H$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.04158</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.022643</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0065925</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.001857</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00052412</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00013833</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Weierstrass</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.025</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$G$3:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.055331</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.013615</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0032334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00091378</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00023754</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00025474</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Cauchy Green</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.025</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0125</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.00625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'L center shrink'!$L$3:$L$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.26797</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29846</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.29828</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29824</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.29823</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.29823</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2129533656"/>
+        <c:axId val="-2129336520"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2129533656"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Edge</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Length</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.457097103103748"/>
+              <c:y val="0.829260325360273"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2129336520"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2129336520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Elastic Energy of Deformation</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.963472299466284"/>
+              <c:y val="0.370860384786807"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2129533656"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="l"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.10997521685254"/>
+          <c:y val="0.424942430545238"/>
+          <c:w val="0.137307052464167"/>
+          <c:h val="0.142096085277076"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Deviation from Target g</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.051696310664716"/>
+          <c:y val="0.162898936170213"/>
+          <c:w val="0.911267605633803"/>
+          <c:h val="0.75531914893617"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Reverse Polar</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.015625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$E$3:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.088113</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.088123</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.090488</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.090007</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.08904</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Weierstrass</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.015625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$D$3:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.15859</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.08142</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.07671</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12261</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1467</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Cauchy Green</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.015625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$F$3:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.47614</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.46847</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.46517</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46328</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.46219</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2124622392"/>
+        <c:axId val="-2121505560"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2124622392"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Edge</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Length</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.444705588789802"/>
+              <c:y val="0.168882978723404"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2121505560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2121505560"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Root Mean Squared Deviation </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.74397518492008E-5"/>
+              <c:y val="0.333124582944081"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2124622392"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="l"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.159531502423263"/>
+          <c:y val="0.707999132523689"/>
+          <c:w val="0.179009355958938"/>
+          <c:h val="0.127645635926865"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Error</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> in Euler-Langrange Equation</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.051696310664716"/>
+          <c:y val="0.162898936170213"/>
+          <c:w val="0.911267605633803"/>
+          <c:h val="0.75531914893617"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Reverse Polar</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.015625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$H$3:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.043544</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.010762</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0026899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00067816</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00017277</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Weierstrass</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.015625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$G$3:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.022629</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.028373</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0013381</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.004188</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.001195</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Cauchy Green</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.015625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$I$3:$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.05639</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.014448</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0036694</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00092602</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00023271</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2121404072"/>
+        <c:axId val="-2121392808"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2121404072"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Edge</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Length</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.444705588789802"/>
+              <c:y val="0.168882978723404"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2121392808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2121392808"/>
+        <c:scaling>
+          <c:logBase val="10.0"/>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Root Mean Squaredd Error </a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.74397518492008E-5"/>
+              <c:y val="0.333124582944081"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2121404072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="l"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.175104022191401"/>
+          <c:y val="0.65715167489657"/>
+          <c:w val="0.153684870095122"/>
+          <c:h val="0.127645635926865"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Elastic Energy</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.051696310664716"/>
+          <c:y val="0.162898936170213"/>
+          <c:w val="0.855505468879587"/>
+          <c:h val="0.75531914893617"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Reverse Polar</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.015625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$H$3:$H$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.043544</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.010762</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0026899</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00067816</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00017277</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Weierstrass</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.015625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$G$3:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.022629</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.028373</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0013381</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.004188</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.001195</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Cauchy Green</c:v>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$B$3:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0625</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.03125</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.015625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'annulus corner squish'!$L$3:$L$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.54755</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5473</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.54722</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.54719</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.54719</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2121424360"/>
+        <c:axId val="-2121381272"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2121424360"/>
+        <c:scaling>
+          <c:orientation val="maxMin"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Edge</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Length</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.457097103103748"/>
+              <c:y val="0.829260325360273"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2121381272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2121381272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="r"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Elastic Energy of Deformation</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.963472299466284"/>
+              <c:y val="0.370860384786807"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2121424360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5009,15 +7161,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>284480</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>314960</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>375920</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>10160</xdr:rowOff>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>162560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5081,6 +7233,208 @@
       <xdr:col>26</xdr:col>
       <xdr:colOff>132080</xdr:colOff>
       <xdr:row>37</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>142240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>497840</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>650240</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>741680</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>10160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>162560</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>10160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>132080</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>142240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>497840</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>650240</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>741680</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>10160</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>162560</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>10160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>132080</xdr:colOff>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>182880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -6039,7 +8393,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="F8" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -6649,8 +9003,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V9"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="A8" sqref="A3:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7259,7 +9613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
@@ -7787,4 +10141,996 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V8"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="6" width="13.1640625" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <f>1/A3</f>
+        <v>0.2</v>
+      </c>
+      <c r="C3">
+        <f>-LOG(A3,2)</f>
+        <v>-2.3219280948873622</v>
+      </c>
+      <c r="D3">
+        <v>0.17194000000000001</v>
+      </c>
+      <c r="E3">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="F3">
+        <v>1.2982</v>
+      </c>
+      <c r="G3">
+        <v>5.5330999999999998E-2</v>
+      </c>
+      <c r="H3">
+        <v>4.1579999999999999E-2</v>
+      </c>
+      <c r="I3">
+        <v>0.13574</v>
+      </c>
+      <c r="J3">
+        <v>7.9823000000000005E-2</v>
+      </c>
+      <c r="K3">
+        <v>2.4107E-2</v>
+      </c>
+      <c r="L3">
+        <v>0.26796999999999999</v>
+      </c>
+      <c r="N3">
+        <f>LOG(D3,2)</f>
+        <v>-2.5400228834712495</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:V8" si="0">LOG(E3,2)</f>
+        <v>-2.8572598278839179</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="0"/>
+        <v>0.37651266128847938</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="0"/>
+        <v>-4.1757681918569212</v>
+      </c>
+      <c r="R3">
+        <f t="shared" si="0"/>
+        <v>-4.5879664315784421</v>
+      </c>
+      <c r="S3">
+        <f t="shared" si="0"/>
+        <v>-2.8810821766500965</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="0"/>
+        <v>-3.647051688878558</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="0"/>
+        <v>-5.3744040641107755</v>
+      </c>
+      <c r="V3">
+        <f>LOG(L3,2)</f>
+        <v>-1.899856598957461</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <f t="shared" ref="B4:B8" si="1">1/A4</f>
+        <v>0.1</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C8" si="2">-LOG(A4,2)</f>
+        <v>-3.3219280948873626</v>
+      </c>
+      <c r="D4">
+        <v>7.8490000000000004E-2</v>
+      </c>
+      <c r="E4">
+        <v>0.12751000000000001</v>
+      </c>
+      <c r="F4">
+        <v>1.2838000000000001</v>
+      </c>
+      <c r="G4">
+        <v>1.3615E-2</v>
+      </c>
+      <c r="H4">
+        <v>2.2643E-2</v>
+      </c>
+      <c r="I4">
+        <v>3.7338999999999997E-2</v>
+      </c>
+      <c r="J4">
+        <v>2.7414000000000001E-2</v>
+      </c>
+      <c r="K4">
+        <v>2.9437999999999999E-2</v>
+      </c>
+      <c r="L4">
+        <v>0.29846</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N8" si="3">LOG(D4,2)</f>
+        <v>-3.6713473302851223</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="0"/>
+        <v>-2.9713176996881252</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="0"/>
+        <v>0.36042046610320916</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>-6.1986592073930158</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="0"/>
+        <v>-5.4647910744320827</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="0"/>
+        <v>-4.7431728994457361</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="0"/>
+        <v>-5.1889433413945696</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="0"/>
+        <v>-5.0861765308830389</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="0"/>
+        <v>-1.7443905023202315</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="2"/>
+        <v>-4.3219280948873626</v>
+      </c>
+      <c r="D5">
+        <v>2.9308000000000001E-2</v>
+      </c>
+      <c r="E5">
+        <v>0.11033</v>
+      </c>
+      <c r="F5">
+        <v>1.2518</v>
+      </c>
+      <c r="G5">
+        <v>3.2334E-3</v>
+      </c>
+      <c r="H5">
+        <v>6.5925000000000003E-3</v>
+      </c>
+      <c r="I5">
+        <v>9.3859000000000008E-3</v>
+      </c>
+      <c r="J5">
+        <v>2.5291000000000001E-2</v>
+      </c>
+      <c r="K5">
+        <v>2.6984000000000001E-2</v>
+      </c>
+      <c r="L5">
+        <v>0.29827999999999999</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="3"/>
+        <v>-5.0925616689847368</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="0"/>
+        <v>-3.1801029651873343</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="0"/>
+        <v>0.32400408139442982</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="0"/>
+        <v>-8.272732292100633</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="0"/>
+        <v>-7.2449586185722525</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="0"/>
+        <v>-6.7352891950899263</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>-5.3052321078341267</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="0"/>
+        <v>-5.2117519663060481</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="0"/>
+        <v>-1.7452608482505727</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="1"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="2"/>
+        <v>-5.3219280948873626</v>
+      </c>
+      <c r="D6">
+        <v>1.1734E-2</v>
+      </c>
+      <c r="E6">
+        <v>0.10804</v>
+      </c>
+      <c r="F6">
+        <v>1.2367999999999999</v>
+      </c>
+      <c r="G6">
+        <v>9.1378E-4</v>
+      </c>
+      <c r="H6">
+        <v>1.8569999999999999E-3</v>
+      </c>
+      <c r="I6">
+        <v>2.3573000000000001E-3</v>
+      </c>
+      <c r="J6">
+        <v>2.4667000000000001E-2</v>
+      </c>
+      <c r="K6">
+        <v>2.6173999999999999E-2</v>
+      </c>
+      <c r="L6">
+        <v>0.29824000000000001</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
+        <v>-6.4131612926528092</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="0"/>
+        <v>-3.2103625499278445</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="0"/>
+        <v>0.30661222437539787</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="0"/>
+        <v>-10.095865513077262</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="0"/>
+        <v>-9.0728104693887541</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="0"/>
+        <v>-8.728648910897693</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>-5.3412739240070906</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="0"/>
+        <v>-5.2557217709605792</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="0"/>
+        <v>-1.7454543297825316</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7">
+        <v>80</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="2"/>
+        <v>-6.3219280948873617</v>
+      </c>
+      <c r="D7">
+        <v>6.0245000000000003E-3</v>
+      </c>
+      <c r="E7">
+        <v>0.10806</v>
+      </c>
+      <c r="F7">
+        <v>1.2296</v>
+      </c>
+      <c r="G7">
+        <v>2.3754000000000001E-4</v>
+      </c>
+      <c r="H7">
+        <v>5.2411999999999999E-4</v>
+      </c>
+      <c r="I7">
+        <v>5.9104000000000003E-4</v>
+      </c>
+      <c r="J7">
+        <v>2.4506E-2</v>
+      </c>
+      <c r="K7">
+        <v>2.5933999999999999E-2</v>
+      </c>
+      <c r="L7">
+        <v>0.29823</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>-7.3749427740171694</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="0"/>
+        <v>-3.2100955078093794</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>0.29818907014132195</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="0"/>
+        <v>-12.039541906347647</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="0"/>
+        <v>-10.897815217434355</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="0"/>
+        <v>-10.72445660811646</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>-5.3507211707314033</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="0"/>
+        <v>-5.2690114484849904</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="0"/>
+        <v>-1.7455027042201738</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8">
+        <v>160</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>6.2500000000000003E-3</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="2"/>
+        <v>-7.3219280948873617</v>
+      </c>
+      <c r="D8">
+        <v>1.6382000000000001E-2</v>
+      </c>
+      <c r="E8">
+        <v>0.10821</v>
+      </c>
+      <c r="F8">
+        <v>1.2262</v>
+      </c>
+      <c r="G8">
+        <v>2.5473999999999999E-4</v>
+      </c>
+      <c r="H8">
+        <v>1.3833000000000001E-4</v>
+      </c>
+      <c r="I8">
+        <v>1.4799999999999999E-4</v>
+      </c>
+      <c r="J8">
+        <v>2.4593E-2</v>
+      </c>
+      <c r="K8">
+        <v>2.5863000000000001E-2</v>
+      </c>
+      <c r="L8">
+        <v>0.29823</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>-5.9317446903084488</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="0"/>
+        <v>-3.2080942659280849</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>0.29419430975931798</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="0"/>
+        <v>-11.938686866067391</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="0"/>
+        <v>-12.819598307965816</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="0"/>
+        <v>-12.722115203695225</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>-5.3456084556081471</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="0"/>
+        <v>-5.272966558319788</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="0"/>
+        <v>-1.7455027042201738</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V7"/>
+  <sheetViews>
+    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="6" width="13.1640625" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B7" si="0">1/A3</f>
+        <v>0.25</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C7" si="1">-LOG(A3,2)</f>
+        <v>-2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.15859000000000001</v>
+      </c>
+      <c r="E3" s="2">
+        <v>8.8112999999999997E-2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>0.47614000000000001</v>
+      </c>
+      <c r="G3" s="2">
+        <v>2.2629E-2</v>
+      </c>
+      <c r="H3" s="2">
+        <v>4.3543999999999999E-2</v>
+      </c>
+      <c r="I3" s="2">
+        <v>5.6390000000000003E-2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.19778000000000001</v>
+      </c>
+      <c r="K3" s="2">
+        <v>0.11987</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0.54754999999999998</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N7" si="2">LOG(D3,2)</f>
+        <v>-2.6566262910916869</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:V7" si="3">LOG(E3,2)</f>
+        <v>-3.5045013028432814</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="3"/>
+        <v>-1.0705422616713658</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="3"/>
+        <v>-5.4656833580164745</v>
+      </c>
+      <c r="R3">
+        <f t="shared" si="3"/>
+        <v>-4.52138224859908</v>
+      </c>
+      <c r="S3">
+        <f t="shared" si="3"/>
+        <v>-4.1484168468234408</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="3"/>
+        <v>-2.3380315502850668</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="3"/>
+        <v>-3.0604574558745807</v>
+      </c>
+      <c r="V3">
+        <f t="shared" si="3"/>
+        <v>-0.86893738321753189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>-3</v>
+      </c>
+      <c r="D4" s="2">
+        <v>8.1420000000000006E-2</v>
+      </c>
+      <c r="E4" s="2">
+        <v>8.8123000000000007E-2</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.46847</v>
+      </c>
+      <c r="G4" s="2">
+        <v>2.8372999999999999E-2</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1.0762000000000001E-2</v>
+      </c>
+      <c r="I4" s="2">
+        <v>1.4448000000000001E-2</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.15706999999999999</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.10718999999999999</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.54730000000000001</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>-3.6184729682968015</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="3"/>
+        <v>-3.5043375797625895</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="3"/>
+        <v>-1.0939714317137053</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="3"/>
+        <v>-5.1393374887112362</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="3"/>
+        <v>-6.5379099778693996</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="3"/>
+        <v>-6.1129863918433163</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="3"/>
+        <v>-2.6705204392981168</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="3"/>
+        <v>-3.2217577751303859</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="3"/>
+        <v>-0.86959623834196109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>-4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>7.671E-2</v>
+      </c>
+      <c r="E5" s="2">
+        <v>9.0487999999999999E-2</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0.46516999999999997</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1.3381000000000001E-3</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2.6898999999999998E-3</v>
+      </c>
+      <c r="I5" s="2">
+        <v>3.6694000000000002E-3</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.13083</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.10365000000000001</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.54722000000000004</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>-3.7044415284740073</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="3"/>
+        <v>-3.4661297068426564</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="3"/>
+        <v>-1.1041700381597284</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="3"/>
+        <v>-9.5455983479703654</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="3"/>
+        <v>-8.5382317446629941</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="3"/>
+        <v>-8.090240103825515</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="3"/>
+        <v>-2.9342346986340493</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="3"/>
+        <v>-3.2702079784400344</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="3"/>
+        <v>-0.86980713554525868</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6">
+        <v>32</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>-5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.12261</v>
+      </c>
+      <c r="E6" s="2">
+        <v>9.0007000000000004E-2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0.46328000000000003</v>
+      </c>
+      <c r="G6" s="2">
+        <v>4.1879999999999999E-3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>6.7816000000000003E-4</v>
+      </c>
+      <c r="I6" s="2">
+        <v>9.2601999999999995E-4</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.16020999999999999</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.1027</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.54718999999999995</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="2"/>
+        <v>-3.027851445694997</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="3"/>
+        <v>-3.473818983081602</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="3"/>
+        <v>-1.1100436929470576</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="3"/>
+        <v>-7.8995228423933659</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="3"/>
+        <v>-10.526086687346966</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="3"/>
+        <v>-10.076669026680324</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="3"/>
+        <v>-2.6419638940811372</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="3"/>
+        <v>-3.2834919132312543</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="3"/>
+        <v>-0.8698862299454152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7">
+        <v>64</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>1.5625E-2</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>-6</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.1467</v>
+      </c>
+      <c r="E7" s="2">
+        <v>8.9039999999999994E-2</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0.46218999999999999</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1.1950000000000001E-3</v>
+      </c>
+      <c r="H7" s="2">
+        <v>1.7276999999999999E-4</v>
+      </c>
+      <c r="I7" s="2">
+        <v>2.3271000000000001E-4</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.16536999999999999</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.10245</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.54718999999999995</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="2"/>
+        <v>-2.7690592238760594</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="3"/>
+        <v>-3.4894025970948528</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="3"/>
+        <v>-1.1134420490724706</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="3"/>
+        <v>-9.7087736664560627</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="3"/>
+        <v>-12.498859651681634</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="3"/>
+        <v>-12.06917917207036</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="3"/>
+        <v>-2.5962305579405012</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="3"/>
+        <v>-3.2870081105382032</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="3"/>
+        <v>-0.8698862299454152</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>